<commit_message>
fix: add access token for GitLab
</commit_message>
<xml_diff>
--- a/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_PMV.xlsx
+++ b/Backend/asset-transfer-basic/application-javascript/blockchain/blockchain_hist_sub_PMV.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,9 +408,23 @@
         <v>a84876e7e0593b0995b09045b34c582c3c6bafc096fb444939e8534553babc53</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <v>16.03.2023</v>
+      </c>
+      <c r="C3" t="str">
+        <v>https://gitlab.intra.infineon.com/digital-reference/process_model_version/-/commit/ed806f827269d7f72e29e68f9f504f8efbab3dc6</v>
+      </c>
+      <c r="D3" t="str">
+        <v>0e08fd8eee36e999283f9dd25c3209735b91da1642e3b67aadf38a56da7ed5d6</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>